<commit_message>
Update key variables in spec
</commit_message>
<xml_diff>
--- a/adam/pk_spec.xlsx
+++ b/adam/pk_spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__transfer\admiral_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E312720-05A6-4A43-ACED-59A8031866C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CEE738-9D1F-42FE-AE1B-6547A672792C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="-105" windowWidth="19425" windowHeight="10995" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="-105" windowWidth="19425" windowHeight="10995" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="527">
   <si>
     <t>Attribute</t>
   </si>
@@ -1639,6 +1639,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>STUDYID, USUBJID, PARAMCD, AVISITN, AFRLT, DTYPE</t>
   </si>
 </sst>
 </file>
@@ -2282,9 +2285,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,7 +2348,7 @@
         <v>48</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>393</v>
+        <v>526</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>394</v>
@@ -2456,7 +2459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
Update for xportr 0.4.0
</commit_message>
<xml_diff>
--- a/adam/pk_spec.xlsx
+++ b/adam/pk_spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__transfer\admiral_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E312720-05A6-4A43-ACED-59A8031866C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F278C5-30C0-448D-B0C4-BCAFF4F4FBB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="-105" windowWidth="19425" windowHeight="10995" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="-105" windowWidth="19425" windowHeight="10995" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="527">
   <si>
     <t>Attribute</t>
   </si>
@@ -1639,6 +1639,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>STUDYID, USUBJID, PARAMCD, AVISITN, AFRLT, DTYPE</t>
   </si>
 </sst>
 </file>
@@ -2282,9 +2285,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,7 +2348,7 @@
         <v>48</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>393</v>
+        <v>526</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>394</v>
@@ -2456,11 +2459,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D125" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C139" sqref="C139"/>
+      <selection pane="bottomRight" activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add PARCAT1 to key variables in spec
</commit_message>
<xml_diff>
--- a/adam/pk_spec.xlsx
+++ b/adam/pk_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__transfer\admiral_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CEE738-9D1F-42FE-AE1B-6547A672792C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBEF4D0-6810-4CE9-834B-166DE82DA18D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="-105" windowWidth="19425" windowHeight="10995" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1641,7 +1641,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>STUDYID, USUBJID, PARAMCD, AVISITN, AFRLT, DTYPE</t>
+    <t>STUDYID, USUBJID, PARAMCD, PARCAT1, AVISITN, AFRLT, DTYPE</t>
   </si>
 </sst>
 </file>
@@ -2460,10 +2460,10 @@
   <dimension ref="A1:R230"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C139" sqref="C139"/>
+      <selection pane="bottomRight" activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add EVID and CMT to key variables for ADPPK
</commit_message>
<xml_diff>
--- a/adam/pk_spec.xlsx
+++ b/adam/pk_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__transfer\admiral_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBEF4D0-6810-4CE9-834B-166DE82DA18D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3CF3A9-0BCC-41B5-BFEB-F625BA483127}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="-105" windowWidth="19425" windowHeight="10995" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1221,9 +1221,6 @@
     <t>BDS-Findings</t>
   </si>
   <si>
-    <t>STUDYID, USUBJID, PARAMCD, AVISITN, AFRLT</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -1642,6 +1639,9 @@
   </si>
   <si>
     <t>STUDYID, USUBJID, PARAMCD, PARCAT1, AVISITN, AFRLT, DTYPE</t>
+  </si>
+  <si>
+    <t>STUDYID, USUBJID, PARAMCD, AVISITN, AFRLT, EVID, CMT</t>
   </si>
 </sst>
 </file>
@@ -2177,7 +2177,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2185,7 +2185,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2193,7 +2193,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2201,7 +2201,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2209,7 +2209,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2287,7 +2287,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,14 +2348,14 @@
         <v>48</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H2"/>
       <c r="I2" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2373,14 +2373,14 @@
         <v>48</v>
       </c>
       <c r="F3" s="18" t="s">
+        <v>526</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>393</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>394</v>
       </c>
       <c r="H3"/>
       <c r="I3" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5270,10 +5270,10 @@
         <v>190</v>
       </c>
       <c r="C124" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D124" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E124" t="s">
         <v>108</v>
@@ -5299,13 +5299,13 @@
         <v>190</v>
       </c>
       <c r="C125" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D125" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E125" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F125">
         <v>8</v>
@@ -5357,13 +5357,13 @@
         <v>190</v>
       </c>
       <c r="C127" t="s">
+        <v>402</v>
+      </c>
+      <c r="D127" t="s">
         <v>403</v>
       </c>
-      <c r="D127" t="s">
+      <c r="E127" t="s">
         <v>404</v>
-      </c>
-      <c r="E127" t="s">
-        <v>405</v>
       </c>
       <c r="F127">
         <v>8</v>
@@ -5371,7 +5371,7 @@
       <c r="H127" s="10"/>
       <c r="I127" s="10"/>
       <c r="J127" s="16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K127" s="10"/>
       <c r="L127" s="10"/>
@@ -5388,13 +5388,13 @@
         <v>190</v>
       </c>
       <c r="C128" t="s">
+        <v>405</v>
+      </c>
+      <c r="D128" t="s">
         <v>406</v>
       </c>
-      <c r="D128" t="s">
-        <v>407</v>
-      </c>
       <c r="E128" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F128">
         <v>8</v>
@@ -5417,13 +5417,13 @@
         <v>190</v>
       </c>
       <c r="C129" t="s">
+        <v>407</v>
+      </c>
+      <c r="D129" t="s">
         <v>408</v>
       </c>
-      <c r="D129" t="s">
-        <v>409</v>
-      </c>
       <c r="E129" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F129">
         <v>8</v>
@@ -5431,7 +5431,7 @@
       <c r="H129" s="10"/>
       <c r="I129" s="10"/>
       <c r="J129" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K129" s="10"/>
       <c r="L129" s="10"/>
@@ -5448,10 +5448,10 @@
         <v>190</v>
       </c>
       <c r="C130" t="s">
+        <v>409</v>
+      </c>
+      <c r="D130" t="s">
         <v>410</v>
-      </c>
-      <c r="D130" t="s">
-        <v>411</v>
       </c>
       <c r="E130" t="s">
         <v>108</v>
@@ -5462,7 +5462,7 @@
       <c r="H130" s="10"/>
       <c r="I130" s="10"/>
       <c r="J130" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K130" s="10"/>
       <c r="L130" s="10"/>
@@ -5508,13 +5508,13 @@
         <v>190</v>
       </c>
       <c r="C132" t="s">
+        <v>411</v>
+      </c>
+      <c r="D132" t="s">
         <v>412</v>
       </c>
-      <c r="D132" t="s">
-        <v>413</v>
-      </c>
       <c r="E132" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F132">
         <v>8</v>
@@ -5566,13 +5566,13 @@
         <v>190</v>
       </c>
       <c r="C134" t="s">
+        <v>413</v>
+      </c>
+      <c r="D134" t="s">
         <v>414</v>
       </c>
-      <c r="D134" t="s">
-        <v>415</v>
-      </c>
       <c r="E134" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F134">
         <v>8</v>
@@ -5624,13 +5624,13 @@
         <v>190</v>
       </c>
       <c r="C136" t="s">
+        <v>415</v>
+      </c>
+      <c r="D136" t="s">
         <v>416</v>
       </c>
-      <c r="D136" t="s">
-        <v>417</v>
-      </c>
       <c r="E136" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F136">
         <v>8</v>
@@ -5653,13 +5653,13 @@
         <v>190</v>
       </c>
       <c r="C137" t="s">
+        <v>417</v>
+      </c>
+      <c r="D137" t="s">
         <v>418</v>
       </c>
-      <c r="D137" t="s">
-        <v>419</v>
-      </c>
       <c r="E137" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F137">
         <v>8</v>
@@ -5685,10 +5685,10 @@
         <v>260</v>
       </c>
       <c r="D138" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E138" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F138">
         <v>8</v>
@@ -5711,10 +5711,10 @@
         <v>190</v>
       </c>
       <c r="C139" t="s">
+        <v>420</v>
+      </c>
+      <c r="D139" t="s">
         <v>421</v>
-      </c>
-      <c r="D139" t="s">
-        <v>422</v>
       </c>
       <c r="E139" t="s">
         <v>108</v>
@@ -5740,13 +5740,13 @@
         <v>190</v>
       </c>
       <c r="C140" t="s">
+        <v>422</v>
+      </c>
+      <c r="D140" t="s">
         <v>423</v>
       </c>
-      <c r="D140" t="s">
-        <v>424</v>
-      </c>
       <c r="E140" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F140">
         <v>8</v>
@@ -5772,10 +5772,10 @@
         <v>258</v>
       </c>
       <c r="D141" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E141" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F141">
         <v>8</v>
@@ -5798,13 +5798,13 @@
         <v>190</v>
       </c>
       <c r="C142" t="s">
+        <v>425</v>
+      </c>
+      <c r="D142" t="s">
         <v>426</v>
       </c>
-      <c r="D142" t="s">
-        <v>427</v>
-      </c>
       <c r="E142" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F142">
         <v>8</v>
@@ -5827,13 +5827,13 @@
         <v>190</v>
       </c>
       <c r="C143" t="s">
+        <v>427</v>
+      </c>
+      <c r="D143" t="s">
         <v>428</v>
       </c>
-      <c r="D143" t="s">
-        <v>429</v>
-      </c>
       <c r="E143" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F143">
         <v>8</v>
@@ -5856,13 +5856,13 @@
         <v>190</v>
       </c>
       <c r="C144" t="s">
+        <v>429</v>
+      </c>
+      <c r="D144" t="s">
         <v>430</v>
       </c>
-      <c r="D144" t="s">
-        <v>431</v>
-      </c>
       <c r="E144" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F144">
         <v>8</v>
@@ -5870,7 +5870,7 @@
       <c r="H144" s="10"/>
       <c r="I144" s="10"/>
       <c r="J144" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K144" s="10"/>
       <c r="L144" s="10"/>
@@ -5887,10 +5887,10 @@
         <v>190</v>
       </c>
       <c r="C145" t="s">
+        <v>431</v>
+      </c>
+      <c r="D145" t="s">
         <v>432</v>
-      </c>
-      <c r="D145" t="s">
-        <v>433</v>
       </c>
       <c r="E145" t="s">
         <v>108</v>
@@ -5901,7 +5901,7 @@
       <c r="H145" s="10"/>
       <c r="I145" s="10"/>
       <c r="J145" s="16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K145" s="10"/>
       <c r="L145" s="10"/>
@@ -5918,13 +5918,13 @@
         <v>190</v>
       </c>
       <c r="C146" t="s">
+        <v>433</v>
+      </c>
+      <c r="D146" t="s">
         <v>434</v>
       </c>
-      <c r="D146" t="s">
-        <v>435</v>
-      </c>
       <c r="E146" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F146">
         <v>8</v>
@@ -5947,10 +5947,10 @@
         <v>190</v>
       </c>
       <c r="C147" t="s">
+        <v>435</v>
+      </c>
+      <c r="D147" t="s">
         <v>436</v>
-      </c>
-      <c r="D147" t="s">
-        <v>437</v>
       </c>
       <c r="E147" t="s">
         <v>108</v>
@@ -5976,13 +5976,13 @@
         <v>190</v>
       </c>
       <c r="C148" t="s">
+        <v>437</v>
+      </c>
+      <c r="D148" t="s">
         <v>438</v>
       </c>
-      <c r="D148" t="s">
-        <v>439</v>
-      </c>
       <c r="E148" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F148">
         <v>8</v>
@@ -5990,7 +5990,7 @@
       <c r="H148" s="10"/>
       <c r="I148" s="10"/>
       <c r="J148" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K148" s="10"/>
       <c r="L148" s="10"/>
@@ -6007,13 +6007,13 @@
         <v>190</v>
       </c>
       <c r="C149" t="s">
+        <v>439</v>
+      </c>
+      <c r="D149" t="s">
         <v>440</v>
       </c>
-      <c r="D149" t="s">
-        <v>441</v>
-      </c>
       <c r="E149" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F149">
         <v>8</v>
@@ -6036,13 +6036,13 @@
         <v>190</v>
       </c>
       <c r="C150" t="s">
+        <v>441</v>
+      </c>
+      <c r="D150" t="s">
         <v>442</v>
       </c>
-      <c r="D150" t="s">
-        <v>443</v>
-      </c>
       <c r="E150" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F150">
         <v>8</v>
@@ -6071,7 +6071,7 @@
         <v>313</v>
       </c>
       <c r="E151" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F151">
         <v>8</v>
@@ -6097,7 +6097,7 @@
         <v>314</v>
       </c>
       <c r="D152" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E152" t="s">
         <v>108</v>
@@ -6123,10 +6123,10 @@
         <v>190</v>
       </c>
       <c r="C153" t="s">
+        <v>444</v>
+      </c>
+      <c r="D153" t="s">
         <v>445</v>
-      </c>
-      <c r="D153" t="s">
-        <v>446</v>
       </c>
       <c r="E153" t="s">
         <v>108</v>
@@ -6152,13 +6152,13 @@
         <v>190</v>
       </c>
       <c r="C154" t="s">
+        <v>446</v>
+      </c>
+      <c r="D154" t="s">
         <v>447</v>
       </c>
-      <c r="D154" t="s">
-        <v>448</v>
-      </c>
       <c r="E154" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F154">
         <v>8</v>
@@ -6181,10 +6181,10 @@
         <v>190</v>
       </c>
       <c r="C155" t="s">
+        <v>448</v>
+      </c>
+      <c r="D155" t="s">
         <v>449</v>
-      </c>
-      <c r="D155" t="s">
-        <v>450</v>
       </c>
       <c r="E155" t="s">
         <v>108</v>
@@ -6201,13 +6201,13 @@
         <v>190</v>
       </c>
       <c r="C156" t="s">
+        <v>450</v>
+      </c>
+      <c r="D156" t="s">
         <v>451</v>
       </c>
-      <c r="D156" t="s">
-        <v>452</v>
-      </c>
       <c r="E156" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F156">
         <v>8</v>
@@ -6221,13 +6221,13 @@
         <v>190</v>
       </c>
       <c r="C157" t="s">
+        <v>452</v>
+      </c>
+      <c r="D157" t="s">
         <v>453</v>
       </c>
-      <c r="D157" t="s">
-        <v>454</v>
-      </c>
       <c r="E157" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F157">
         <v>8</v>
@@ -6244,10 +6244,10 @@
         <v>272</v>
       </c>
       <c r="D158" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E158" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F158">
         <v>8</v>
@@ -6261,13 +6261,13 @@
         <v>190</v>
       </c>
       <c r="C159" t="s">
+        <v>455</v>
+      </c>
+      <c r="D159" t="s">
         <v>456</v>
       </c>
-      <c r="D159" t="s">
-        <v>457</v>
-      </c>
       <c r="E159" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F159">
         <v>8</v>
@@ -6281,13 +6281,13 @@
         <v>190</v>
       </c>
       <c r="C160" t="s">
+        <v>457</v>
+      </c>
+      <c r="D160" t="s">
         <v>458</v>
       </c>
-      <c r="D160" t="s">
-        <v>459</v>
-      </c>
       <c r="E160" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F160">
         <v>8</v>
@@ -6301,13 +6301,13 @@
         <v>190</v>
       </c>
       <c r="C161" t="s">
+        <v>459</v>
+      </c>
+      <c r="D161" t="s">
         <v>460</v>
       </c>
-      <c r="D161" t="s">
-        <v>461</v>
-      </c>
       <c r="E161" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F161">
         <v>8</v>
@@ -6321,10 +6321,10 @@
         <v>190</v>
       </c>
       <c r="C162" t="s">
+        <v>461</v>
+      </c>
+      <c r="D162" t="s">
         <v>462</v>
-      </c>
-      <c r="D162" t="s">
-        <v>463</v>
       </c>
       <c r="E162" t="s">
         <v>108</v>
@@ -6341,19 +6341,19 @@
         <v>190</v>
       </c>
       <c r="C163" t="s">
+        <v>463</v>
+      </c>
+      <c r="D163" t="s">
         <v>464</v>
       </c>
-      <c r="D163" t="s">
-        <v>465</v>
-      </c>
       <c r="E163" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F163">
         <v>8</v>
       </c>
       <c r="J163" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
@@ -6364,7 +6364,7 @@
         <v>190</v>
       </c>
       <c r="C164" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D164" t="s">
         <v>86</v>
@@ -6384,19 +6384,19 @@
         <v>190</v>
       </c>
       <c r="C165" t="s">
+        <v>466</v>
+      </c>
+      <c r="D165" t="s">
         <v>467</v>
       </c>
-      <c r="D165" t="s">
-        <v>468</v>
-      </c>
       <c r="E165" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F165">
         <v>8</v>
       </c>
       <c r="J165" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
@@ -6407,19 +6407,19 @@
         <v>190</v>
       </c>
       <c r="C166" t="s">
+        <v>468</v>
+      </c>
+      <c r="D166" t="s">
         <v>469</v>
       </c>
-      <c r="D166" t="s">
-        <v>470</v>
-      </c>
       <c r="E166" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F166">
         <v>8</v>
       </c>
       <c r="J166" s="15" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
@@ -6430,10 +6430,10 @@
         <v>190</v>
       </c>
       <c r="C167" t="s">
+        <v>470</v>
+      </c>
+      <c r="D167" t="s">
         <v>471</v>
-      </c>
-      <c r="D167" t="s">
-        <v>472</v>
       </c>
       <c r="E167" t="s">
         <v>108</v>
@@ -6442,7 +6442,7 @@
         <v>40</v>
       </c>
       <c r="J167" s="15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
@@ -6453,10 +6453,10 @@
         <v>190</v>
       </c>
       <c r="C168" t="s">
+        <v>472</v>
+      </c>
+      <c r="D168" t="s">
         <v>473</v>
-      </c>
-      <c r="D168" t="s">
-        <v>474</v>
       </c>
       <c r="E168" t="s">
         <v>108</v>
@@ -6476,10 +6476,10 @@
         <v>372</v>
       </c>
       <c r="D169" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E169" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F169">
         <v>8</v>
@@ -6496,10 +6496,10 @@
         <v>374</v>
       </c>
       <c r="D170" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E170" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F170">
         <v>8</v>
@@ -6516,10 +6516,10 @@
         <v>376</v>
       </c>
       <c r="D171" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E171" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F171">
         <v>8</v>
@@ -6533,13 +6533,13 @@
         <v>190</v>
       </c>
       <c r="C172" t="s">
+        <v>477</v>
+      </c>
+      <c r="D172" t="s">
         <v>478</v>
       </c>
-      <c r="D172" t="s">
-        <v>479</v>
-      </c>
       <c r="E172" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F172">
         <v>8</v>
@@ -6556,10 +6556,10 @@
         <v>65</v>
       </c>
       <c r="D173" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E173" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F173">
         <v>8</v>
@@ -6596,19 +6596,19 @@
         <v>190</v>
       </c>
       <c r="C175" t="s">
+        <v>480</v>
+      </c>
+      <c r="D175" t="s">
         <v>481</v>
       </c>
-      <c r="D175" t="s">
-        <v>482</v>
-      </c>
       <c r="E175" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F175">
         <v>8</v>
       </c>
       <c r="J175" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
@@ -6642,19 +6642,19 @@
         <v>190</v>
       </c>
       <c r="C177" t="s">
+        <v>482</v>
+      </c>
+      <c r="D177" t="s">
         <v>483</v>
       </c>
-      <c r="D177" t="s">
-        <v>484</v>
-      </c>
       <c r="E177" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F177">
         <v>8</v>
       </c>
       <c r="J177" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
@@ -6665,10 +6665,10 @@
         <v>190</v>
       </c>
       <c r="C178" t="s">
+        <v>484</v>
+      </c>
+      <c r="D178" t="s">
         <v>485</v>
-      </c>
-      <c r="D178" t="s">
-        <v>486</v>
       </c>
       <c r="E178" t="s">
         <v>108</v>
@@ -6677,7 +6677,7 @@
         <v>100</v>
       </c>
       <c r="J178" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
@@ -6688,19 +6688,19 @@
         <v>190</v>
       </c>
       <c r="C179" t="s">
+        <v>486</v>
+      </c>
+      <c r="D179" t="s">
         <v>487</v>
       </c>
-      <c r="D179" t="s">
-        <v>488</v>
-      </c>
       <c r="E179" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F179">
         <v>8</v>
       </c>
       <c r="J179" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
@@ -6731,13 +6731,13 @@
         <v>190</v>
       </c>
       <c r="C181" t="s">
+        <v>488</v>
+      </c>
+      <c r="D181" t="s">
         <v>489</v>
       </c>
-      <c r="D181" t="s">
-        <v>490</v>
-      </c>
       <c r="E181" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F181">
         <v>8</v>
@@ -6774,10 +6774,10 @@
         <v>190</v>
       </c>
       <c r="C183" t="s">
+        <v>490</v>
+      </c>
+      <c r="D183" t="s">
         <v>491</v>
-      </c>
-      <c r="D183" t="s">
-        <v>492</v>
       </c>
       <c r="E183" t="s">
         <v>108</v>
@@ -6786,7 +6786,7 @@
         <v>100</v>
       </c>
       <c r="J183" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
@@ -6797,19 +6797,19 @@
         <v>190</v>
       </c>
       <c r="C184" t="s">
+        <v>492</v>
+      </c>
+      <c r="D184" t="s">
         <v>493</v>
       </c>
-      <c r="D184" t="s">
-        <v>494</v>
-      </c>
       <c r="E184" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F184">
         <v>8</v>
       </c>
       <c r="J184" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
@@ -6820,13 +6820,13 @@
         <v>190</v>
       </c>
       <c r="C185" t="s">
+        <v>494</v>
+      </c>
+      <c r="D185" t="s">
         <v>495</v>
       </c>
-      <c r="D185" t="s">
-        <v>496</v>
-      </c>
       <c r="E185" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F185">
         <v>8</v>
@@ -6840,13 +6840,13 @@
         <v>190</v>
       </c>
       <c r="C186" t="s">
+        <v>496</v>
+      </c>
+      <c r="D186" t="s">
         <v>497</v>
       </c>
-      <c r="D186" t="s">
-        <v>498</v>
-      </c>
       <c r="E186" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F186">
         <v>8</v>
@@ -6860,13 +6860,13 @@
         <v>190</v>
       </c>
       <c r="C187" t="s">
+        <v>498</v>
+      </c>
+      <c r="D187" t="s">
         <v>499</v>
       </c>
-      <c r="D187" t="s">
-        <v>500</v>
-      </c>
       <c r="E187" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F187">
         <v>8</v>
@@ -6880,13 +6880,13 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
+        <v>500</v>
+      </c>
+      <c r="D188" t="s">
         <v>501</v>
       </c>
-      <c r="D188" t="s">
-        <v>502</v>
-      </c>
       <c r="E188" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F188">
         <v>8</v>
@@ -6900,13 +6900,13 @@
         <v>190</v>
       </c>
       <c r="C189" t="s">
+        <v>502</v>
+      </c>
+      <c r="D189" t="s">
         <v>503</v>
       </c>
-      <c r="D189" t="s">
-        <v>504</v>
-      </c>
       <c r="E189" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F189">
         <v>8</v>
@@ -6920,13 +6920,13 @@
         <v>190</v>
       </c>
       <c r="C190" t="s">
+        <v>504</v>
+      </c>
+      <c r="D190" t="s">
         <v>505</v>
       </c>
-      <c r="D190" t="s">
-        <v>506</v>
-      </c>
       <c r="E190" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F190">
         <v>8</v>
@@ -7351,20 +7351,20 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5" t="s">
@@ -7373,20 +7373,20 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E8" s="3">
         <v>2</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="5" t="s">
@@ -7395,20 +7395,20 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E9" s="3">
         <v>3</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="5" t="s">
@@ -7417,20 +7417,20 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E10" s="3">
         <v>4</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6" t="s">
@@ -7527,20 +7527,20 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="5" t="s">
@@ -7551,20 +7551,20 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E16" s="3">
         <v>2</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="5" t="s">
@@ -7575,20 +7575,20 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E17" s="3">
         <v>3</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="5" t="s">
@@ -7599,20 +7599,20 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E18" s="2">
         <v>4</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="5" t="s">
@@ -7623,10 +7623,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="5" t="s">
@@ -7647,10 +7647,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="5" t="s">
@@ -7671,10 +7671,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="5" t="s">
@@ -7695,10 +7695,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="5" t="s">
@@ -7741,10 +7741,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
@@ -7754,7 +7754,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5" t="s">
@@ -7763,20 +7763,20 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="23" t="s">
@@ -7851,10 +7851,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>118</v>
@@ -7877,10 +7877,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>118</v>
@@ -7903,20 +7903,20 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="5" t="s">
@@ -7925,20 +7925,20 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E32" s="3">
         <v>2</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="5" t="s">
@@ -8299,22 +8299,22 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>122</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E47" s="14">
         <v>1</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G47" s="15" t="s">
         <v>169</v>
@@ -8325,22 +8325,22 @@
     </row>
     <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>122</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E48" s="14">
         <v>2</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G48" s="15" t="s">
         <v>170</v>
@@ -8351,22 +8351,22 @@
     </row>
     <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>122</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E49" s="14">
         <v>3</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G49" s="15" t="s">
         <v>171</v>
@@ -8377,22 +8377,22 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>122</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E50" s="14">
         <v>4</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G50" s="15" t="s">
         <v>172</v>
@@ -8481,19 +8481,19 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E54" s="14">
         <v>1</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H54" s="15" t="s">
         <v>154</v>
@@ -8501,19 +8501,19 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E55" s="14">
         <v>2</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H55" s="15" t="s">
         <v>155</v>
@@ -8521,19 +8521,19 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E56" s="14">
         <v>3</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H56" s="15" t="s">
         <v>156</v>
@@ -8620,39 +8620,39 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E60" s="14">
         <v>1</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E61" s="14">
         <v>1</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H61" s="15" t="s">
         <v>135</v>
@@ -8660,19 +8660,19 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E62" s="14">
         <v>1</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G62" s="15" t="s">
         <v>165</v>
@@ -8695,10 +8695,10 @@
         <v>1</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H63" s="15" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -8715,10 +8715,10 @@
         <v>2</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -8729,16 +8729,16 @@
         <v>254</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E65" s="14">
         <v>1</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -8749,64 +8749,64 @@
         <v>254</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E66" s="14">
         <v>2</v>
       </c>
       <c r="F66" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E67" s="14">
         <v>1</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E68" s="14">
         <v>1</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D69" s="15" t="s">
         <v>108</v>
@@ -8815,18 +8815,18 @@
         <v>1</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D70" s="15" t="s">
         <v>108</v>
@@ -8835,30 +8835,30 @@
         <v>1</v>
       </c>
       <c r="F70" s="15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E71" s="14">
         <v>1</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -8906,16 +8906,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" t="s">
         <v>396</v>
       </c>
-      <c r="B2" t="s">
-        <v>397</v>
-      </c>
       <c r="C2" t="s">
         <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>